<commit_message>
Document citation style updated.
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -51,6 +51,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Texas is annexed into the United States as the 28</t>
     </r>
@@ -60,6 +61,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -68,6 +70,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> state in the Union (December 29, 1845)</t>
     </r>
@@ -108,6 +111,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Private Lawrence Sullivan Ross elected Major in the 6</t>
     </r>
@@ -117,6 +121,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -125,6 +130,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Regiment of Texas Cavalry by his peers</t>
     </r>
@@ -147,6 +153,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">13</t>
     </r>
@@ -156,6 +163,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -164,6 +172,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Amendment to the US Constitution is adopted, formally abolishing slavery (December 18, 1865)</t>
     </r>
@@ -211,6 +220,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -232,6 +242,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -309,7 +320,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,7 +533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>1891</v>
       </c>
@@ -541,7 +552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>1898</v>
       </c>

</xml_diff>

<commit_message>
Document reorganized and timeline added.
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -20,27 +20,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t xml:space="preserve">year</t>
   </si>
   <si>
-    <t xml:space="preserve">national or state history</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross family and personal history</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texas A&amp;M History</t>
+    <t xml:space="preserve">state or national history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR family and personal history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latex sources</t>
   </si>
   <si>
     <t xml:space="preserve">sources</t>
   </si>
   <si>
-    <t xml:space="preserve">Texas revolution begins (October 2, 1835)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Battle of the Alamo (February 23 through March 6, 1836)</t>
+    <t xml:space="preserve">Texas revolution begins 
+(October 2, 1835)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Battle of the Alamo 
+(February 23 through March 6, 1836)</t>
   </si>
   <si>
     <t xml:space="preserve">Texas Declaration of Independence is adopted (March 2, 1836)</t>
@@ -76,7 +78,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross is born to Shapely Ross and Catherine Fulkerson in Iowa (September 27, 1838)</t>
+    <t xml:space="preserve">LSR is born to Shapely Ross and Catherine Fulkerson in Iowa (September 27, 1838)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\cite{rosspapersummary}</t>
   </si>
   <si>
     <t xml:space="preserve">Ross family papers description webpage</t>
@@ -85,16 +90,19 @@
     <t xml:space="preserve">Shapely Ross runs to Texas after physical altercation with a lawyer over a runaway slave (sometime in 1838). Catherine Fulkerson follows with rest of family shortly after. </t>
   </si>
   <si>
+    <t xml:space="preserve">\cite[pg. 53]{page}</t>
+  </si>
+  <si>
     <t xml:space="preserve">William Page document (pg 53-54)</t>
   </si>
   <si>
     <t xml:space="preserve">Ross family moves to Waco permanently (1849)</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross graduates from Wesleyan University in Alabama (1859)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross resigns from active duty Texas Ranger service (1861; immediately before U.S. Civil War begins, but no date given)</t>
+    <t xml:space="preserve">LSR graduates from Wesleyan University in Alabama (1859)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR resigns from active duty Texas Ranger service (1861; immediately before U.S. Civil War begins, but no date given)</t>
   </si>
   <si>
     <t xml:space="preserve">Ross family papers description webpage; see also pg 43 of William Page document</t>
@@ -103,49 +111,37 @@
     <t xml:space="preserve">United States Civil War begins (April 12, 1861)</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross marries Elizabeth Dorothy Tinsley (May 28, 1861)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Private Lawrence Sullivan Ross elected Major in the 6</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Regiment of Texas Cavalry by his peers</t>
-    </r>
+    <t xml:space="preserve">LSR marries Elizabeth Dorothy Tinsley (May 28, 1861)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private LSR elected Major in the 6th Regiment of Texas Cavalry by his peers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\cite[pg. 36 and 37]{texasbrigade}</t>
   </si>
   <si>
     <t xml:space="preserve">Ross Texas Brigade document, page 36-37</t>
   </si>
   <si>
+    <t xml:space="preserve">Battle of Antietam (September 17, 1862). Bloodiest day in US military history with 22,717 dead, wounded, or missing.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emancipation Proclamation issued by President Abraham Lincoln (January 1, 1863)</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross promoted to Brigadier General (December 1863). Ross was 25 years of age. Ross commanded a cavalry brigade in the Army of Tennessee.</t>
+    <t xml:space="preserve">Battle of Gettysburg (July 1 thru 3, 1863)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR promoted to Brigadier General (December 1863). Ross was 25 years of age. Ross commanded a cavalry brigade in the Army of Tennessee.</t>
   </si>
   <si>
     <t xml:space="preserve">United States Civil War ends (April 9, 1865)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">President Abraham Lincoln is shot by John Wilkes Booth (April 14, 1865) and dies shortly after (April 15, 1865)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Union general Gordon Granger reads ‘General Order No. 3’ to the public in Galvaston, TX, announcing total emancipation of those held as slaves (June 18, 1865; commonly known as Juneteenth)</t>
   </si>
   <si>
     <r>
@@ -178,31 +174,34 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross elected sheriff of McLennan County, Texas (1873)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross attends the Texas Constitutional Convention as a delegate from Central Texas (1876)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross elected Texas state senator, going on to serve one term (1880)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross becomes Governor of Texas (January 18, 1887). Ross would go on to serve two terms as governor, leaving office January 20, 1891. </t>
+    <t xml:space="preserve">LSR elected sheriff of McLennan County, Texas (1873)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR attends the Texas Constitutional Convention as a delegate from Central Texas (1876)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR elected Texas state senator, going on to serve one term (1880)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR becomes Governor of Texas (January 18, 1887). Ross would go on to serve two terms as governor, leaving office January 20, 1891. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">\cite{tsl}</t>
   </si>
   <si>
     <t xml:space="preserve">tsl.texas.gov</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapely Ross, father to Lawrence Sullivan Ross, dies (September 17, 1889)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross leaves the office of the Governor of the State of Texas (January 20, 1891</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross accepts position as President of the Agricultural and Mechanical College of Texas (1891)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence Sullivan Ross dies at home (January 3, 1898). Ross was still college president at the time. </t>
+    <t xml:space="preserve">Shapely Ross, father to LSR, dies (September 17, 1889)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR leaves the office of the Governor of the State of Texas (January 20, 1891</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR accepts position as President of the Agricultural and Mechanical College of Texas (1891)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR dies at home (January 3, 1898). Ross was still college president at the time. </t>
   </si>
   <si>
     <t xml:space="preserve">https://tshaonline.org/handbook/online/articles/fro81</t>
@@ -317,13 +316,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="27.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="2" width="32.4"/>
@@ -364,11 +363,17 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1836</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>1836</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -380,16 +385,25 @@
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>1838</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -397,10 +411,13 @@
         <v>1849</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -408,10 +425,13 @@
         <v>1859</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -419,10 +439,13 @@
         <v>1861</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -430,137 +453,217 @@
         <v>1861</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>1861</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>1861</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="49.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
+        <v>1862</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="49.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
         <v>1863</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="49.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
+        <v>1863</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>1863</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
         <v>1865</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>1865</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>1865</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>1865</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
         <v>1873</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
         <v>1876</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="C23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
         <v>1880</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="C24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
         <v>1887</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="C25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
         <v>1889</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="C26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
         <v>1891</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="C27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>1891</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
         <v>1898</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>34</v>
+      <c r="C29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2nd round of edits complete.
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t xml:space="preserve">Texas Declaration of Independence is adopted (March 2, 1836)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR is born to Shapely Ross and Catherine Fulkerson in Iowa (September 27, 1838)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\cite{rosspapersummary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ross family papers description webpage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shapely Ross runs to Texas after physical altercation with a lawyer over a runaway slave (sometime in 1838). Catherine Fulkerson follows with rest of family shortly after. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">\cite[pg. 53]{page}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William Page document (pg 53-54)</t>
   </si>
   <si>
     <r>
@@ -76,24 +94,6 @@
       </rPr>
       <t xml:space="preserve"> state in the Union (December 29, 1845)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">LSR is born to Shapely Ross and Catherine Fulkerson in Iowa (September 27, 1838)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\cite{rosspapersummary}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ross family papers description webpage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shapely Ross runs to Texas after physical altercation with a lawyer over a runaway slave (sometime in 1838). Catherine Fulkerson follows with rest of family shortly after. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">\cite[pg. 53]{page}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">William Page document (pg 53-54)</t>
   </si>
   <si>
     <t xml:space="preserve">Ross family moves to Waco permanently (1849)</t>
@@ -318,8 +318,8 @@
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -372,37 +372,37 @@
     </row>
     <row r="5" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>1836</v>
-      </c>
-      <c r="B5" s="2" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>1838</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>1838</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -414,10 +414,10 @@
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -428,10 +428,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -442,7 +442,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>18</v>
@@ -464,10 +464,10 @@
         <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -516,10 +516,10 @@
         <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -562,10 +562,10 @@
         <v>32</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -576,10 +576,10 @@
         <v>33</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -590,10 +590,10 @@
         <v>34</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,10 +618,10 @@
         <v>38</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,10 +646,10 @@
         <v>40</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,7 +660,7 @@
         <v>41</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Corrected Shapley Ross spelling.
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -48,7 +48,7 @@
     <t xml:space="preserve">Texas Declaration of Independence is adopted (March 2, 1836)</t>
   </si>
   <si>
-    <t xml:space="preserve">LSR is born to Shapely Ross and Catherine Fulkerson in Iowa (September 27, 1838)</t>
+    <t xml:space="preserve">LSR is born to Shapley Ross and Catherine Fulkerson in Iowa (September 27, 1838)</t>
   </si>
   <si>
     <t xml:space="preserve">\cite{rosspapersummary}</t>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Ross family papers description webpage</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapely Ross runs to Texas after physical altercation with a lawyer over a runaway slave (sometime in 1838). Catherine Fulkerson follows with rest of family shortly after. </t>
+    <t xml:space="preserve">Shapley Ross runs to Texas after physical altercation with a lawyer over a runaway slave (sometime in 1838). Catherine Fulkerson follows with rest of family shortly after. </t>
   </si>
   <si>
     <t xml:space="preserve">\cite[pg. 53]{page}</t>
@@ -192,7 +192,7 @@
     <t xml:space="preserve">tsl.texas.gov</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapely Ross, father to LSR, dies (September 17, 1889)</t>
+    <t xml:space="preserve">Shapley Ross, father to LSR, dies (September 17, 1889)</t>
   </si>
   <si>
     <t xml:space="preserve">LSR leaves the office of the Governor of the State of Texas (January 20, 1891</t>
@@ -319,7 +319,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>